<commit_message>
Atualizando o Backlog e o gráfico Burndown
</commit_message>
<xml_diff>
--- a/Backlog/Backlog - Grupo 04.xlsx
+++ b/Backlog/Backlog - Grupo 04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMINI~1\AppData\Local\Temp\MicrosoftEdgeDownloads\1ba27438-4a72-4323-a5d7-010fb8d88998\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E60C97-C49B-488F-851F-CD9DA5AAE116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6ACDE4-9E97-496C-B0BC-E52A083BE7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
   <si>
     <t>Configuração e instalação do Arduino Uno R3 com Sensor MQ-2 utilizando Protoboard e 3 Jumpers (Macho-Macho).</t>
   </si>
@@ -391,20 +391,23 @@
     <t>Deixar o site responsivo para os mais diversos dispositivos (navegadores e mobile)</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Peso Planejado</t>
-  </si>
-  <si>
-    <t>Peso Realizado</t>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Pontos Planejados</t>
+  </si>
+  <si>
+    <t>Pontos Realizados</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,8 +439,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,8 +467,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -483,11 +506,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,29 +608,140 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCB0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -550,7 +759,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -608,107 +821,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFCB0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFCB0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -936,6 +1048,26 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCB0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -975,12 +1107,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -989,16 +1118,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" b="1"/>
-              <a:t>Burndown</a:t>
+              <a:t>BURNDOW</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" b="1" baseline="0"/>
-              <a:t> Sprints</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.5833333333333117E-3"/>
+          <c:y val="1.3888888888888888E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1012,12 +1144,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1030,20 +1159,30 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0914260717410318E-2"/>
+          <c:y val="0.24520888013998252"/>
+          <c:w val="0.89019685039370078"/>
+          <c:h val="0.67053988043161272"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndow!$B$1</c:f>
+              <c:f>Burndow!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Peso Planejado</c:v>
+                  <c:v>TOTAL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1051,41 +1190,71 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$B$3,Burndow!$B$5:$B$7)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndow!$B$2:$B$4</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$B$3,Burndow!$B$5:$B$7)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,7 +1262,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2AA3-47BA-AB1A-1AF6FFA88514}"/>
+              <c16:uniqueId val="{00000000-DB02-4BC6-89C5-6B53B65CC9FC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1102,11 +1271,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndow!$C$1</c:f>
+              <c:f>Burndow!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Peso Realizado</c:v>
+                  <c:v>Pontos Planejados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1121,111 +1290,425 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8166666666666691E-2"/>
+                  <c:y val="-5.7835739282589678E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2611111111111113E-2"/>
+                  <c:y val="3.01272236803732E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0944444444444445E-2"/>
+                  <c:y val="2.5497594050743571E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$B$3,Burndow!$B$5:$B$7)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndow!$C$2:$C$4</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$C$3:$C$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$C$3,Burndow!$C$5:$C$7)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2AA3-47BA-AB1A-1AF6FFA88514}"/>
+              <c16:uniqueId val="{00000001-DB02-4BC6-89C5-6B53B65CC9FC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1109385935"/>
-        <c:axId val="1109387855"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1109385935"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:rich>
+            <c:strRef>
+              <c:f>Burndow!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pontos Realizados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0944444444444445E-2"/>
+                  <c:y val="3.9386482939632504E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3500000000000002E-2"/>
+                  <c:y val="3.4756853310002833E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5388888888888888E-2"/>
+                  <c:y val="-3.0057961504811985E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2611111111111113E-2"/>
+                  <c:y val="-3.4687591134441531E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR" sz="1200" b="1"/>
-                  <a:t>Sprints</a:t>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$B$3,Burndow!$B$5:$B$7)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Burndow!$D$3:$D$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Burndow!$D$3,Burndow!$D$5:$D$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DB02-4BC6-89C5-6B53B65CC9FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1937044160"/>
+        <c:axId val="1937044640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1937044160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1247,12 +1730,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1262,7 +1742,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1109387855"/>
+        <c:crossAx val="1937044640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1270,26 +1750,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1109387855"/>
+        <c:axId val="1937044640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1306,12 +1772,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1321,7 +1784,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1109385935"/>
+        <c:crossAx val="1937044160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1339,10 +1802,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20984886264216973"/>
-          <c:y val="0.89375218722659666"/>
-          <c:w val="0.62689982502187225"/>
-          <c:h val="7.8996427529892096E-2"/>
+          <c:x val="0.67850743657042856"/>
+          <c:y val="2.3726305045202681E-2"/>
+          <c:w val="0.32076268591426071"/>
+          <c:h val="0.25868110236220471"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1358,12 +1821,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1375,7 +1835,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1402,7 +1862,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr>
+        <a:defRPr sz="1050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
           <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
@@ -1459,7 +1922,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1567,6 +2030,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1577,6 +2045,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1608,6 +2081,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1965,23 +2441,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>250825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>415925</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B5948F8-B567-5851-5C67-1A2C893CFF9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D256309-5BFF-F5B8-B78D-38A11A8B76F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2479,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
     <sortCondition ref="G3:G43"/>
@@ -2029,12 +2505,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:C5" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" headerRowBorderDxfId="1" tableBorderDxfId="11">
+  <autoFilter ref="B4:D7" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Peso Planejado" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{7731B8CD-B998-43D0-A8D9-2AC97939B511}" name="Peso Realizado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2305,13 +2781,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
     <col min="3" max="7" width="19.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
@@ -2325,48 +2801,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3993,25 +4469,25 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:J51 C3:F51">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+  <conditionalFormatting sqref="C3:F51 H3:J51">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J51">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4048,72 +4524,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72880F1E-8FC6-43CF-9104-1D9717B6A027}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="11"/>
+    <col min="1" max="1" width="4.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="13">
+        <f>SUM(C5:C7)</f>
+        <v>351</v>
+      </c>
+      <c r="D3" s="14">
+        <f>SUM(D5:D7)</f>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C4" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D4" s="17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13">
-        <f>SUMIF(Backlog!$G:$G,A2,Backlog!$E:$E)</f>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>117</v>
+      </c>
+      <c r="D5" s="9">
+        <f>SUMIF(Backlog!$G:$G,B5,Backlog!$E:$E)</f>
         <v>95</v>
       </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="13">
-        <f>SUMIF(Backlog!$G:$G,A3,Backlog!$E:$E)</f>
+      <c r="C6" s="9">
+        <v>117</v>
+      </c>
+      <c r="D6" s="9">
+        <f>SUMIF(Backlog!$G:$G,B6,Backlog!$E:$E)</f>
         <v>124</v>
       </c>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
-        <f>SUMIF(Backlog!$G:$G,A4,Backlog!$E:$E)</f>
+      <c r="C7" s="9">
+        <v>117</v>
+      </c>
+      <c r="D7" s="9">
+        <f>SUMIF(Backlog!$G:$G,B7,Backlog!$E:$E)</f>
         <v>133</v>
       </c>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="13">
-        <f>SUM(B2:B4)</f>
-        <v>352</v>
-      </c>
-      <c r="C5" s="13">
-        <f>SUM(C2:C4)</f>
-        <v>0</v>
+      <c r="C9" s="18">
+        <f>D3/3</f>
+        <v>117.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações na Modelagem de Dados e Backlog
</commit_message>
<xml_diff>
--- a/Backlog/Backlog - Grupo 04.xlsx
+++ b/Backlog/Backlog - Grupo 04.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMINI~1\AppData\Local\Temp\MicrosoftEdgeDownloads\1ba27438-4a72-4323-a5d7-010fb8d88998\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6ACDE4-9E97-496C-B0BC-E52A083BE7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E06AC7-92BA-4B49-A933-764A93914A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,12 +614,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,47 +635,17 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFCB0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -821,6 +785,42 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCB0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2480,7 +2480,19 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
+  <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Em Andamento"/>
+        <filter val="Pendente"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
     <sortCondition ref="G3:G43"/>
     <sortCondition ref="C3:C43"/>
@@ -2505,12 +2517,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" headerRowBorderDxfId="1" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="B4:D7" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2782,7 +2794,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2801,18 +2813,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -2846,7 +2858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2879,7 +2891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2912,7 +2924,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2945,7 +2957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="62" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2978,7 +2990,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3012,7 +3024,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3045,7 +3057,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3091,7 @@
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -3112,7 +3124,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3145,7 +3157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3178,7 +3190,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3211,7 +3223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3334,7 +3346,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>106</v>
@@ -3367,7 +3379,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>104</v>
@@ -3376,7 +3388,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>103</v>
@@ -3409,7 +3421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -3442,7 +3454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -3475,7 +3487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3541,7 +3553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -3574,7 +3586,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -3598,7 +3610,7 @@
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>103</v>
@@ -3607,7 +3619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>102</v>
@@ -3640,7 +3652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -3673,7 +3685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3697,7 +3709,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>107</v>
@@ -3730,7 +3742,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>104</v>
@@ -3772,7 +3784,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -3796,7 +3808,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>106</v>
@@ -3871,7 +3883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -3904,7 +3916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -3937,7 +3949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -3970,7 +3982,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -4003,7 +4015,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -4036,7 +4048,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -4069,7 +4081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -4102,7 +4114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
@@ -4135,7 +4147,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -4168,7 +4180,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -4201,7 +4213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4234,7 +4246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4267,7 +4279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -4300,7 +4312,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -4333,7 +4345,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
@@ -4366,7 +4378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
@@ -4399,7 +4411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
@@ -4432,7 +4444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -4470,24 +4482,24 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:F51 H3:J51">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J51">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4541,26 +4553,26 @@
   <sheetData>
     <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <f>SUM(C5:C7)</f>
         <v>351</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <f>SUM(D5:D7)</f>
         <v>352</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4602,10 +4614,10 @@
     </row>
     <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <f>D3/3</f>
         <v>117.33333333333333</v>
       </c>

</xml_diff>